<commit_message>
working with ratios and some multiples
</commit_message>
<xml_diff>
--- a/BABA_2025-05-14.xlsx
+++ b/BABA_2025-05-14.xlsx
@@ -10,13 +10,15 @@
     <sheet name="income_statement" sheetId="1" r:id="rId1"/>
     <sheet name="cashflow_statement" sheetId="2" r:id="rId2"/>
     <sheet name="balancesheet_statement" sheetId="3" r:id="rId3"/>
+    <sheet name="ratios" sheetId="4" r:id="rId4"/>
+    <sheet name="multiples" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="223">
   <si>
     <t>LTM</t>
   </si>
@@ -165,7 +167,7 @@
     <t>Effective Tax Rate %</t>
   </si>
   <si>
-    <t>BABA</t>
+    <t>baba</t>
   </si>
   <si>
     <t>Depreciation &amp; Amortization</t>
@@ -469,6 +471,222 @@
   </si>
   <si>
     <t>Full Time Employees</t>
+  </si>
+  <si>
+    <t>Return on Assets %</t>
+  </si>
+  <si>
+    <t>Return on Capital %</t>
+  </si>
+  <si>
+    <t>Return On Equity %</t>
+  </si>
+  <si>
+    <t>Return on Common Equity %</t>
+  </si>
+  <si>
+    <t>Gross Profit Margin %</t>
+  </si>
+  <si>
+    <t>SG&amp;A Margin %</t>
+  </si>
+  <si>
+    <t>EBITDA Margin %</t>
+  </si>
+  <si>
+    <t>EBITA Margin %</t>
+  </si>
+  <si>
+    <t>EBIT Margin %</t>
+  </si>
+  <si>
+    <t>Income From Continuing Operations Margin %</t>
+  </si>
+  <si>
+    <t>Net Income Margin %</t>
+  </si>
+  <si>
+    <t>Normalized Net Income Margin %</t>
+  </si>
+  <si>
+    <t>Net Avail. For Common Margin %</t>
+  </si>
+  <si>
+    <t>Levered Free Cash Flow Margin %</t>
+  </si>
+  <si>
+    <t>Unlevered Free Cash Flow Margin %</t>
+  </si>
+  <si>
+    <t>Asset Turnover</t>
+  </si>
+  <si>
+    <t>Fixed Assets Turnover</t>
+  </si>
+  <si>
+    <t>Receivables Turnover</t>
+  </si>
+  <si>
+    <t>Inventory Turnover</t>
+  </si>
+  <si>
+    <t>Working Capital Turnover</t>
+  </si>
+  <si>
+    <t>Current Ratio</t>
+  </si>
+  <si>
+    <t>Quick Ratio</t>
+  </si>
+  <si>
+    <t>Op Cash Flow to Current Liab</t>
+  </si>
+  <si>
+    <t>Avg. Cash Conversion Cycle</t>
+  </si>
+  <si>
+    <t>Avg. Days Sales Outstanding</t>
+  </si>
+  <si>
+    <t>Avg. Days Outstanding Inventory</t>
+  </si>
+  <si>
+    <t>Avg. Days Payable Outstanding</t>
+  </si>
+  <si>
+    <t>Total Debt / Equity</t>
+  </si>
+  <si>
+    <t>Total Debt / Capital</t>
+  </si>
+  <si>
+    <t>Total Liabilities / Total Assets</t>
+  </si>
+  <si>
+    <t>EBIT / Interest Expense</t>
+  </si>
+  <si>
+    <t>EBITDA / Interest Expense</t>
+  </si>
+  <si>
+    <t>(EBITDA - Capex) / Interest Expense</t>
+  </si>
+  <si>
+    <t>FFO Interest Coverage</t>
+  </si>
+  <si>
+    <t>FFO to Total Debt (x)</t>
+  </si>
+  <si>
+    <t>Total Debt / EBITDA</t>
+  </si>
+  <si>
+    <t>Net Debt / EBITDA</t>
+  </si>
+  <si>
+    <t>Net Debt / (EBITDA - Capex)</t>
+  </si>
+  <si>
+    <t>NTM Total Enterprise Value / Revenues</t>
+  </si>
+  <si>
+    <t>NTM Price / Sales (P/S)</t>
+  </si>
+  <si>
+    <t>NTM Total Enterprise Value / EBITDA</t>
+  </si>
+  <si>
+    <t>NTM Total Enterprise Value / EBIT</t>
+  </si>
+  <si>
+    <t>NTM Price / Normalized Earnings (P/E)</t>
+  </si>
+  <si>
+    <t>NTM Market Cap / Free Cash Flow</t>
+  </si>
+  <si>
+    <t>NTM Levered Free Cash Flow Yield</t>
+  </si>
+  <si>
+    <t>LTM Total Enterprise Value / Revenues</t>
+  </si>
+  <si>
+    <t>LTM Price / Sales (P/S)</t>
+  </si>
+  <si>
+    <t>LTM Total Enterprise Value / Gross Profit</t>
+  </si>
+  <si>
+    <t>LTM Total Enterprise Value / EBITDA</t>
+  </si>
+  <si>
+    <t>LTM Total Enterprise Value / EBIT</t>
+  </si>
+  <si>
+    <t>LTM Price / Diluted EPS Before Extra</t>
+  </si>
+  <si>
+    <t>LTM Price / Book Value per Share</t>
+  </si>
+  <si>
+    <t>LTM Price / Tangible Book Value per Share</t>
+  </si>
+  <si>
+    <t>LTM Total Enterprise Value / Unlevered Free Cash Flow</t>
+  </si>
+  <si>
+    <t>LTM Market Cap / Levered Free Cash Flow</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Total Enterprise Value (MM)</t>
+  </si>
+  <si>
+    <t>Market Cap (MM)</t>
+  </si>
+  <si>
+    <t>NTM Revenues</t>
+  </si>
+  <si>
+    <t>NTM EBITDA</t>
+  </si>
+  <si>
+    <t>NTM EBIT</t>
+  </si>
+  <si>
+    <t>NTM Normalized Earnings Per Share</t>
+  </si>
+  <si>
+    <t>NTM Levered Free Cash Flow</t>
+  </si>
+  <si>
+    <t>LTM Revenues</t>
+  </si>
+  <si>
+    <t>LTM Gross Profit</t>
+  </si>
+  <si>
+    <t>LTM EBITDA</t>
+  </si>
+  <si>
+    <t>LTM EBIT</t>
+  </si>
+  <si>
+    <t>LTM Diluted EPS Before Extra</t>
+  </si>
+  <si>
+    <t>LTM Book Value per Share</t>
+  </si>
+  <si>
+    <t>LTM Tangible Book Value per Share</t>
+  </si>
+  <si>
+    <t>LTM Unlevered Free Cash Flow</t>
+  </si>
+  <si>
+    <t>LTM Levered Free Cash Flow</t>
   </si>
 </sst>
 </file>
@@ -6801,4 +7019,2232 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="45.7109375" customWidth="1"/>
+    <col min="2" max="38" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2012</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2013</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="L1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="M1" s="1">
+        <v>2023</v>
+      </c>
+      <c r="N1" s="1">
+        <v>2024</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2">
+        <v>16.2314</v>
+      </c>
+      <c r="D2">
+        <v>18.702</v>
+      </c>
+      <c r="E2">
+        <v>7.9397</v>
+      </c>
+      <c r="F2">
+        <v>5.9621</v>
+      </c>
+      <c r="G2">
+        <v>7.019</v>
+      </c>
+      <c r="H2">
+        <v>7.2112</v>
+      </c>
+      <c r="I2">
+        <v>4.5777</v>
+      </c>
+      <c r="J2">
+        <v>5.242</v>
+      </c>
+      <c r="K2">
+        <v>4.5615</v>
+      </c>
+      <c r="L2">
+        <v>3.5625</v>
+      </c>
+      <c r="M2">
+        <v>3.8787</v>
+      </c>
+      <c r="N2">
+        <v>4.929</v>
+      </c>
+      <c r="O2">
+        <v>5.0403</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3">
+        <v>14.2742</v>
+      </c>
+      <c r="C3">
+        <v>32.2409</v>
+      </c>
+      <c r="D3">
+        <v>31.2625</v>
+      </c>
+      <c r="E3">
+        <v>10.8671</v>
+      </c>
+      <c r="F3">
+        <v>9.425700000000001</v>
+      </c>
+      <c r="G3">
+        <v>11.557</v>
+      </c>
+      <c r="H3">
+        <v>12.1466</v>
+      </c>
+      <c r="I3">
+        <v>8.0488</v>
+      </c>
+      <c r="J3">
+        <v>8.9214</v>
+      </c>
+      <c r="K3">
+        <v>8.273199999999999</v>
+      </c>
+      <c r="L3">
+        <v>7.3076</v>
+      </c>
+      <c r="M3">
+        <v>7.7529</v>
+      </c>
+      <c r="N3">
+        <v>10.1163</v>
+      </c>
+      <c r="O3">
+        <v>10.4787</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4">
+        <v>38.1492</v>
+      </c>
+      <c r="D4">
+        <v>90.60209999999999</v>
+      </c>
+      <c r="E4">
+        <v>24.5515</v>
+      </c>
+      <c r="F4">
+        <v>35.0355</v>
+      </c>
+      <c r="G4">
+        <v>14.4483</v>
+      </c>
+      <c r="H4">
+        <v>16.2129</v>
+      </c>
+      <c r="I4">
+        <v>15.3554</v>
+      </c>
+      <c r="J4">
+        <v>18.8612</v>
+      </c>
+      <c r="K4">
+        <v>14.5963</v>
+      </c>
+      <c r="L4">
+        <v>4.3474</v>
+      </c>
+      <c r="M4">
+        <v>5.9473</v>
+      </c>
+      <c r="N4">
+        <v>6.3816</v>
+      </c>
+      <c r="O4">
+        <v>10.2736</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5">
+        <v>53.4197</v>
+      </c>
+      <c r="D5">
+        <v>157.4401</v>
+      </c>
+      <c r="E5">
+        <v>27.634</v>
+      </c>
+      <c r="F5">
+        <v>39.4342</v>
+      </c>
+      <c r="G5">
+        <v>17.6184</v>
+      </c>
+      <c r="H5">
+        <v>19.8519</v>
+      </c>
+      <c r="I5">
+        <v>20.4177</v>
+      </c>
+      <c r="J5">
+        <v>23.9269</v>
+      </c>
+      <c r="K5">
+        <v>17.7577</v>
+      </c>
+      <c r="L5">
+        <v>6.5705</v>
+      </c>
+      <c r="M5">
+        <v>7.4823</v>
+      </c>
+      <c r="N5">
+        <v>8.0701</v>
+      </c>
+      <c r="O5">
+        <v>11.9656</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6">
+        <v>67.2709</v>
+      </c>
+      <c r="C6">
+        <v>71.8428</v>
+      </c>
+      <c r="D6">
+        <v>74.5371</v>
+      </c>
+      <c r="E6">
+        <v>68.7234</v>
+      </c>
+      <c r="F6">
+        <v>66.03319999999999</v>
+      </c>
+      <c r="G6">
+        <v>62.9589</v>
+      </c>
+      <c r="H6">
+        <v>57.5479</v>
+      </c>
+      <c r="I6">
+        <v>45.8433</v>
+      </c>
+      <c r="J6">
+        <v>45.1232</v>
+      </c>
+      <c r="K6">
+        <v>41.5135</v>
+      </c>
+      <c r="L6">
+        <v>36.8504</v>
+      </c>
+      <c r="M6">
+        <v>36.8515</v>
+      </c>
+      <c r="N6">
+        <v>37.7026</v>
+      </c>
+      <c r="O6">
+        <v>38.8085</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B7">
+        <v>26.3121</v>
+      </c>
+      <c r="C7">
+        <v>18.837</v>
+      </c>
+      <c r="D7">
+        <v>14.2731</v>
+      </c>
+      <c r="E7">
+        <v>21.407</v>
+      </c>
+      <c r="F7">
+        <v>20.2801</v>
+      </c>
+      <c r="G7">
+        <v>18.0403</v>
+      </c>
+      <c r="H7">
+        <v>17.3974</v>
+      </c>
+      <c r="I7">
+        <v>16.7151</v>
+      </c>
+      <c r="J7">
+        <v>15.4734</v>
+      </c>
+      <c r="K7">
+        <v>16.5226</v>
+      </c>
+      <c r="L7">
+        <v>17.7854</v>
+      </c>
+      <c r="M7">
+        <v>16.77</v>
+      </c>
+      <c r="N7">
+        <v>16.6947</v>
+      </c>
+      <c r="O7">
+        <v>18.8023</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B8">
+        <v>29.9875</v>
+      </c>
+      <c r="C8">
+        <v>44.3462</v>
+      </c>
+      <c r="D8">
+        <v>53.0302</v>
+      </c>
+      <c r="E8">
+        <v>36.435</v>
+      </c>
+      <c r="F8">
+        <v>36.1211</v>
+      </c>
+      <c r="G8">
+        <v>39.8659</v>
+      </c>
+      <c r="H8">
+        <v>36.9582</v>
+      </c>
+      <c r="I8">
+        <v>26.1492</v>
+      </c>
+      <c r="J8">
+        <v>27.0276</v>
+      </c>
+      <c r="K8">
+        <v>21.958</v>
+      </c>
+      <c r="L8">
+        <v>16.9462</v>
+      </c>
+      <c r="M8">
+        <v>17.7218</v>
+      </c>
+      <c r="N8">
+        <v>19.4675</v>
+      </c>
+      <c r="O8">
+        <v>19.4005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9">
+        <v>26.4918</v>
+      </c>
+      <c r="C9">
+        <v>42.1328</v>
+      </c>
+      <c r="D9">
+        <v>50.5637</v>
+      </c>
+      <c r="E9">
+        <v>33.4405</v>
+      </c>
+      <c r="F9">
+        <v>32.4639</v>
+      </c>
+      <c r="G9">
+        <v>36.5949</v>
+      </c>
+      <c r="H9">
+        <v>33.5003</v>
+      </c>
+      <c r="I9">
+        <v>22.2171</v>
+      </c>
+      <c r="J9">
+        <v>23.0401</v>
+      </c>
+      <c r="K9">
+        <v>18.2791</v>
+      </c>
+      <c r="L9">
+        <v>13.6864</v>
+      </c>
+      <c r="M9">
+        <v>14.5216</v>
+      </c>
+      <c r="N9">
+        <v>16.6369</v>
+      </c>
+      <c r="O9">
+        <v>16.6574</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B10">
+        <v>25.7178</v>
+      </c>
+      <c r="C10">
+        <v>41.7562</v>
+      </c>
+      <c r="D10">
+        <v>49.9638</v>
+      </c>
+      <c r="E10">
+        <v>30.5889</v>
+      </c>
+      <c r="F10">
+        <v>29.2229</v>
+      </c>
+      <c r="G10">
+        <v>30.9035</v>
+      </c>
+      <c r="H10">
+        <v>28.2135</v>
+      </c>
+      <c r="I10">
+        <v>16.3478</v>
+      </c>
+      <c r="J10">
+        <v>18.7427</v>
+      </c>
+      <c r="K10">
+        <v>15.2789</v>
+      </c>
+      <c r="L10">
+        <v>11.3118</v>
+      </c>
+      <c r="M10">
+        <v>12.3184</v>
+      </c>
+      <c r="N10">
+        <v>14.7389</v>
+      </c>
+      <c r="O10">
+        <v>15.0975</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B11">
+        <v>23.2958</v>
+      </c>
+      <c r="C11">
+        <v>25.0572</v>
+      </c>
+      <c r="D11">
+        <v>44.5737</v>
+      </c>
+      <c r="E11">
+        <v>31.9143</v>
+      </c>
+      <c r="F11">
+        <v>70.4833</v>
+      </c>
+      <c r="G11">
+        <v>26.0473</v>
+      </c>
+      <c r="H11">
+        <v>24.5386</v>
+      </c>
+      <c r="I11">
+        <v>21.291</v>
+      </c>
+      <c r="J11">
+        <v>27.5352</v>
+      </c>
+      <c r="K11">
+        <v>19.9757</v>
+      </c>
+      <c r="L11">
+        <v>5.5188</v>
+      </c>
+      <c r="M11">
+        <v>7.5485</v>
+      </c>
+      <c r="N11">
+        <v>7.579</v>
+      </c>
+      <c r="O11">
+        <v>11.7056</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12">
+        <v>21.1136</v>
+      </c>
+      <c r="C12">
+        <v>24.7182</v>
+      </c>
+      <c r="D12">
+        <v>44.4061</v>
+      </c>
+      <c r="E12">
+        <v>31.8369</v>
+      </c>
+      <c r="F12">
+        <v>70.6524</v>
+      </c>
+      <c r="G12">
+        <v>27.5947</v>
+      </c>
+      <c r="H12">
+        <v>25.6099</v>
+      </c>
+      <c r="I12">
+        <v>23.3215</v>
+      </c>
+      <c r="J12">
+        <v>29.3172</v>
+      </c>
+      <c r="K12">
+        <v>20.9926</v>
+      </c>
+      <c r="L12">
+        <v>7.2971</v>
+      </c>
+      <c r="M12">
+        <v>8.378500000000001</v>
+      </c>
+      <c r="N12">
+        <v>8.500999999999999</v>
+      </c>
+      <c r="O12">
+        <v>12.316</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B13">
+        <v>15.4269</v>
+      </c>
+      <c r="C13">
+        <v>24.5907</v>
+      </c>
+      <c r="D13">
+        <v>33.0584</v>
+      </c>
+      <c r="E13">
+        <v>25.2747</v>
+      </c>
+      <c r="F13">
+        <v>49.7232</v>
+      </c>
+      <c r="G13">
+        <v>23.6053</v>
+      </c>
+      <c r="H13">
+        <v>21.2762</v>
+      </c>
+      <c r="I13">
+        <v>18.8327</v>
+      </c>
+      <c r="J13">
+        <v>22.016</v>
+      </c>
+      <c r="K13">
+        <v>17.7881</v>
+      </c>
+      <c r="L13">
+        <v>10.3104</v>
+      </c>
+      <c r="M13">
+        <v>7.942</v>
+      </c>
+      <c r="N13">
+        <v>9.501200000000001</v>
+      </c>
+      <c r="O13">
+        <v>11.8118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B14">
+        <v>21.1136</v>
+      </c>
+      <c r="C14">
+        <v>24.3474</v>
+      </c>
+      <c r="D14">
+        <v>43.9509</v>
+      </c>
+      <c r="E14">
+        <v>31.6899</v>
+      </c>
+      <c r="F14">
+        <v>70.6524</v>
+      </c>
+      <c r="G14">
+        <v>27.5947</v>
+      </c>
+      <c r="H14">
+        <v>25.5667</v>
+      </c>
+      <c r="I14">
+        <v>23.2456</v>
+      </c>
+      <c r="J14">
+        <v>29.2838</v>
+      </c>
+      <c r="K14">
+        <v>20.955</v>
+      </c>
+      <c r="L14">
+        <v>7.2631</v>
+      </c>
+      <c r="M14">
+        <v>8.3469</v>
+      </c>
+      <c r="N14">
+        <v>8.4725</v>
+      </c>
+      <c r="O14">
+        <v>12.2593</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C15">
+        <v>33.3476</v>
+      </c>
+      <c r="D15">
+        <v>19.7518</v>
+      </c>
+      <c r="E15">
+        <v>52.4683</v>
+      </c>
+      <c r="F15">
+        <v>36.9436</v>
+      </c>
+      <c r="G15">
+        <v>37.8141</v>
+      </c>
+      <c r="H15">
+        <v>35.8394</v>
+      </c>
+      <c r="I15">
+        <v>25.2481</v>
+      </c>
+      <c r="J15">
+        <v>22.3756</v>
+      </c>
+      <c r="K15">
+        <v>26.0152</v>
+      </c>
+      <c r="L15">
+        <v>7.3284</v>
+      </c>
+      <c r="M15">
+        <v>13.1257</v>
+      </c>
+      <c r="N15">
+        <v>13.0402</v>
+      </c>
+      <c r="O15">
+        <v>9.8041</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C16">
+        <v>36.1941</v>
+      </c>
+      <c r="D16">
+        <v>22.2433</v>
+      </c>
+      <c r="E16">
+        <v>54.7238</v>
+      </c>
+      <c r="F16">
+        <v>38.1461</v>
+      </c>
+      <c r="G16">
+        <v>38.8689</v>
+      </c>
+      <c r="H16">
+        <v>36.7299</v>
+      </c>
+      <c r="I16">
+        <v>26.1088</v>
+      </c>
+      <c r="J16">
+        <v>23.0108</v>
+      </c>
+      <c r="K16">
+        <v>26.4052</v>
+      </c>
+      <c r="L16">
+        <v>7.6881</v>
+      </c>
+      <c r="M16">
+        <v>13.5515</v>
+      </c>
+      <c r="N16">
+        <v>13.568</v>
+      </c>
+      <c r="O16">
+        <v>10.3947</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B17">
+        <v>0.424168</v>
+      </c>
+      <c r="C17">
+        <v>0.541137</v>
+      </c>
+      <c r="D17">
+        <v>0.470681</v>
+      </c>
+      <c r="E17">
+        <v>0.298331</v>
+      </c>
+      <c r="F17">
+        <v>0.277678</v>
+      </c>
+      <c r="G17">
+        <v>0.312291</v>
+      </c>
+      <c r="H17">
+        <v>0.348985</v>
+      </c>
+      <c r="I17">
+        <v>0.390481</v>
+      </c>
+      <c r="J17">
+        <v>0.388207</v>
+      </c>
+      <c r="K17">
+        <v>0.424376</v>
+      </c>
+      <c r="L17">
+        <v>0.503117</v>
+      </c>
+      <c r="M17">
+        <v>0.49553</v>
+      </c>
+      <c r="N17">
+        <v>0.533291</v>
+      </c>
+      <c r="O17">
+        <v>0.529264</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C18">
+        <v>11.008451</v>
+      </c>
+      <c r="D18">
+        <v>11.184151</v>
+      </c>
+      <c r="E18">
+        <v>10.353804</v>
+      </c>
+      <c r="F18">
+        <v>8.884662000000001</v>
+      </c>
+      <c r="G18">
+        <v>9.355578</v>
+      </c>
+      <c r="H18">
+        <v>5.773481</v>
+      </c>
+      <c r="I18">
+        <v>4.754559</v>
+      </c>
+      <c r="J18">
+        <v>4.430786</v>
+      </c>
+      <c r="K18">
+        <v>4.012816</v>
+      </c>
+      <c r="L18">
+        <v>3.63538</v>
+      </c>
+      <c r="M18">
+        <v>3.451841</v>
+      </c>
+      <c r="N18">
+        <v>3.651143</v>
+      </c>
+      <c r="O18">
+        <v>4.80741</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C19">
+        <v>154.09375</v>
+      </c>
+      <c r="D19">
+        <v>39.373078</v>
+      </c>
+      <c r="E19">
+        <v>18.278723</v>
+      </c>
+      <c r="F19">
+        <v>19.53699</v>
+      </c>
+      <c r="G19">
+        <v>24.417309</v>
+      </c>
+      <c r="H19">
+        <v>20.957668</v>
+      </c>
+      <c r="I19">
+        <v>20.603827</v>
+      </c>
+      <c r="J19">
+        <v>19.592589</v>
+      </c>
+      <c r="K19">
+        <v>21.014839</v>
+      </c>
+      <c r="L19">
+        <v>20.692581</v>
+      </c>
+      <c r="M19">
+        <v>20.16053</v>
+      </c>
+      <c r="N19">
+        <v>23.494252</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="H20">
+        <v>38.690094</v>
+      </c>
+      <c r="I20">
+        <v>31.232075</v>
+      </c>
+      <c r="J20">
+        <v>23.914247</v>
+      </c>
+      <c r="K20">
+        <v>19.641688</v>
+      </c>
+      <c r="L20">
+        <v>18.593666</v>
+      </c>
+      <c r="M20">
+        <v>18.711396</v>
+      </c>
+      <c r="N20">
+        <v>21.712852</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B21">
+        <v>1.240091</v>
+      </c>
+      <c r="C21">
+        <v>1.800855</v>
+      </c>
+      <c r="D21">
+        <v>1.724325</v>
+      </c>
+      <c r="E21">
+        <v>0.74391</v>
+      </c>
+      <c r="F21">
+        <v>1.233511</v>
+      </c>
+      <c r="G21">
+        <v>1.792446</v>
+      </c>
+      <c r="H21">
+        <v>2.067545</v>
+      </c>
+      <c r="I21">
+        <v>6.019487</v>
+      </c>
+      <c r="J21">
+        <v>2.305852</v>
+      </c>
+      <c r="K21">
+        <v>2.696554</v>
+      </c>
+      <c r="L21">
+        <v>3.34861</v>
+      </c>
+      <c r="M21">
+        <v>2.778775</v>
+      </c>
+      <c r="N21">
+        <v>2.840344</v>
+      </c>
+      <c r="O21">
+        <v>4.452801</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B22">
+        <v>2.37418</v>
+      </c>
+      <c r="C22">
+        <v>1.798791</v>
+      </c>
+      <c r="D22">
+        <v>1.814492</v>
+      </c>
+      <c r="E22">
+        <v>3.582098</v>
+      </c>
+      <c r="F22">
+        <v>2.575664</v>
+      </c>
+      <c r="G22">
+        <v>1.943739</v>
+      </c>
+      <c r="H22">
+        <v>1.891281</v>
+      </c>
+      <c r="I22">
+        <v>1.30146</v>
+      </c>
+      <c r="J22">
+        <v>1.913917</v>
+      </c>
+      <c r="K22">
+        <v>1.704906</v>
+      </c>
+      <c r="L22">
+        <v>1.663787</v>
+      </c>
+      <c r="M22">
+        <v>1.811247</v>
+      </c>
+      <c r="N22">
+        <v>1.786124</v>
+      </c>
+      <c r="O22">
+        <v>1.482078</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B23">
+        <v>1.961109</v>
+      </c>
+      <c r="C23">
+        <v>1.402375</v>
+      </c>
+      <c r="D23">
+        <v>1.278942</v>
+      </c>
+      <c r="E23">
+        <v>3.426245</v>
+      </c>
+      <c r="F23">
+        <v>2.441322</v>
+      </c>
+      <c r="G23">
+        <v>1.831505</v>
+      </c>
+      <c r="H23">
+        <v>1.731544</v>
+      </c>
+      <c r="I23">
+        <v>1.120027</v>
+      </c>
+      <c r="J23">
+        <v>1.682046</v>
+      </c>
+      <c r="K23">
+        <v>1.431977</v>
+      </c>
+      <c r="L23">
+        <v>1.37138</v>
+      </c>
+      <c r="M23">
+        <v>1.527474</v>
+      </c>
+      <c r="N23">
+        <v>1.518197</v>
+      </c>
+      <c r="O23">
+        <v>0.991077</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B24">
+        <v>0.7892940000000001</v>
+      </c>
+      <c r="C24">
+        <v>0.6032920000000001</v>
+      </c>
+      <c r="D24">
+        <v>0.705622</v>
+      </c>
+      <c r="E24">
+        <v>1.038944</v>
+      </c>
+      <c r="F24">
+        <v>1.09218</v>
+      </c>
+      <c r="G24">
+        <v>0.885532</v>
+      </c>
+      <c r="H24">
+        <v>0.92633</v>
+      </c>
+      <c r="I24">
+        <v>0.726998</v>
+      </c>
+      <c r="J24">
+        <v>0.746704</v>
+      </c>
+      <c r="K24">
+        <v>0.614233</v>
+      </c>
+      <c r="L24">
+        <v>0.371977</v>
+      </c>
+      <c r="M24">
+        <v>0.518363</v>
+      </c>
+      <c r="N24">
+        <v>0.43319</v>
+      </c>
+      <c r="O24">
+        <v>0.348367</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="H25">
+        <v>-73.73511000000001</v>
+      </c>
+      <c r="I25">
+        <v>-51.56793</v>
+      </c>
+      <c r="J25">
+        <v>-42.232008</v>
+      </c>
+      <c r="K25">
+        <v>-32.21052</v>
+      </c>
+      <c r="L25">
+        <v>-30.73738</v>
+      </c>
+      <c r="M25">
+        <v>-36.105435</v>
+      </c>
+      <c r="N25">
+        <v>-43.28133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C26">
+        <v>2.368485</v>
+      </c>
+      <c r="D26">
+        <v>9.27027</v>
+      </c>
+      <c r="E26">
+        <v>19.96842</v>
+      </c>
+      <c r="F26">
+        <v>18.733344</v>
+      </c>
+      <c r="G26">
+        <v>14.94821</v>
+      </c>
+      <c r="H26">
+        <v>17.415975</v>
+      </c>
+      <c r="I26">
+        <v>17.71491</v>
+      </c>
+      <c r="J26">
+        <v>18.680274</v>
+      </c>
+      <c r="K26">
+        <v>17.368525</v>
+      </c>
+      <c r="L26">
+        <v>17.63899</v>
+      </c>
+      <c r="M26">
+        <v>18.104365</v>
+      </c>
+      <c r="N26">
+        <v>15.578058</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="H27">
+        <v>9.43379</v>
+      </c>
+      <c r="I27">
+        <v>11.68657</v>
+      </c>
+      <c r="J27">
+        <v>15.304656</v>
+      </c>
+      <c r="K27">
+        <v>18.58288</v>
+      </c>
+      <c r="L27">
+        <v>19.630065</v>
+      </c>
+      <c r="M27">
+        <v>19.506695</v>
+      </c>
+      <c r="N27">
+        <v>16.85613</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E28">
+        <v>55.16172</v>
+      </c>
+      <c r="F28">
+        <v>71.83628400000001</v>
+      </c>
+      <c r="H28">
+        <v>100.584875</v>
+      </c>
+      <c r="I28">
+        <v>80.96941</v>
+      </c>
+      <c r="J28">
+        <v>76.216938</v>
+      </c>
+      <c r="K28">
+        <v>68.161925</v>
+      </c>
+      <c r="L28">
+        <v>68.006435</v>
+      </c>
+      <c r="M28">
+        <v>73.71649499999999</v>
+      </c>
+      <c r="N28">
+        <v>75.715518</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B29">
+        <v>3.7314</v>
+      </c>
+      <c r="C29">
+        <v>302.0164</v>
+      </c>
+      <c r="D29">
+        <v>100.9188</v>
+      </c>
+      <c r="E29">
+        <v>33.4108</v>
+      </c>
+      <c r="F29">
+        <v>23.0689</v>
+      </c>
+      <c r="G29">
+        <v>28.5654</v>
+      </c>
+      <c r="H29">
+        <v>28.7676</v>
+      </c>
+      <c r="I29">
+        <v>22.0676</v>
+      </c>
+      <c r="J29">
+        <v>16.7437</v>
+      </c>
+      <c r="K29">
+        <v>16.7435</v>
+      </c>
+      <c r="L29">
+        <v>16.3184</v>
+      </c>
+      <c r="M29">
+        <v>17.416</v>
+      </c>
+      <c r="N29">
+        <v>18.4805</v>
+      </c>
+      <c r="O29">
+        <v>24.1415</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B30">
+        <v>3.556</v>
+      </c>
+      <c r="C30">
+        <v>74.0448</v>
+      </c>
+      <c r="D30">
+        <v>48.95</v>
+      </c>
+      <c r="E30">
+        <v>24.5189</v>
+      </c>
+      <c r="F30">
+        <v>18.3579</v>
+      </c>
+      <c r="G30">
+        <v>21.6746</v>
+      </c>
+      <c r="H30">
+        <v>21.5985</v>
+      </c>
+      <c r="I30">
+        <v>17.5463</v>
+      </c>
+      <c r="J30">
+        <v>13.7543</v>
+      </c>
+      <c r="K30">
+        <v>13.6969</v>
+      </c>
+      <c r="L30">
+        <v>13.3735</v>
+      </c>
+      <c r="M30">
+        <v>14.1692</v>
+      </c>
+      <c r="N30">
+        <v>14.9949</v>
+      </c>
+      <c r="O30">
+        <v>18.685</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B31">
+        <v>27.17</v>
+      </c>
+      <c r="C31">
+        <v>82.8175</v>
+      </c>
+      <c r="D31">
+        <v>63.5128</v>
+      </c>
+      <c r="E31">
+        <v>38.3742</v>
+      </c>
+      <c r="F31">
+        <v>31.4914</v>
+      </c>
+      <c r="G31">
+        <v>36.6374</v>
+      </c>
+      <c r="H31">
+        <v>39.1405</v>
+      </c>
+      <c r="I31">
+        <v>36.9393</v>
+      </c>
+      <c r="J31">
+        <v>33.0037</v>
+      </c>
+      <c r="K31">
+        <v>35.8879</v>
+      </c>
+      <c r="L31">
+        <v>36.1746</v>
+      </c>
+      <c r="M31">
+        <v>35.9445</v>
+      </c>
+      <c r="N31">
+        <v>36.9571</v>
+      </c>
+      <c r="O31">
+        <v>40.9802</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B32">
+        <v>75.735294</v>
+      </c>
+      <c r="C32">
+        <v>9.168575000000001</v>
+      </c>
+      <c r="D32">
+        <v>12.533683</v>
+      </c>
+      <c r="E32">
+        <v>8.476362999999999</v>
+      </c>
+      <c r="F32">
+        <v>15.188591</v>
+      </c>
+      <c r="G32">
+        <v>18.312242</v>
+      </c>
+      <c r="H32">
+        <v>19.800616</v>
+      </c>
+      <c r="I32">
+        <v>11.870134</v>
+      </c>
+      <c r="J32">
+        <v>18.442857</v>
+      </c>
+      <c r="K32">
+        <v>24.484807</v>
+      </c>
+      <c r="L32">
+        <v>19.65716</v>
+      </c>
+      <c r="M32">
+        <v>18.081953</v>
+      </c>
+      <c r="N32">
+        <v>17.455391</v>
+      </c>
+      <c r="O32">
+        <v>15.977471</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B33">
+        <v>88.308823</v>
+      </c>
+      <c r="C33">
+        <v>9.737277000000001</v>
+      </c>
+      <c r="D33">
+        <v>13.302914</v>
+      </c>
+      <c r="E33">
+        <v>10.096363</v>
+      </c>
+      <c r="F33">
+        <v>18.773895</v>
+      </c>
+      <c r="G33">
+        <v>23.622987</v>
+      </c>
+      <c r="H33">
+        <v>25.937745</v>
+      </c>
+      <c r="I33">
+        <v>18.986897</v>
+      </c>
+      <c r="J33">
+        <v>27.676254</v>
+      </c>
+      <c r="K33">
+        <v>36.710232</v>
+      </c>
+      <c r="L33">
+        <v>31.855978</v>
+      </c>
+      <c r="M33">
+        <v>27.952179</v>
+      </c>
+      <c r="N33">
+        <v>24.490877</v>
+      </c>
+      <c r="O33">
+        <v>21.755389</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B34">
+        <v>56.42647</v>
+      </c>
+      <c r="C34">
+        <v>8.145038</v>
+      </c>
+      <c r="D34">
+        <v>11.021022</v>
+      </c>
+      <c r="E34">
+        <v>7.294545</v>
+      </c>
+      <c r="F34">
+        <v>13.200924</v>
+      </c>
+      <c r="G34">
+        <v>19.502433</v>
+      </c>
+      <c r="H34">
+        <v>20.433538</v>
+      </c>
+      <c r="I34">
+        <v>12.150289</v>
+      </c>
+      <c r="J34">
+        <v>21.392471</v>
+      </c>
+      <c r="K34">
+        <v>27.449731</v>
+      </c>
+      <c r="L34">
+        <v>20.996536</v>
+      </c>
+      <c r="M34">
+        <v>22.151233</v>
+      </c>
+      <c r="N34">
+        <v>20.453252</v>
+      </c>
+      <c r="O34">
+        <v>18.29662</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B35">
+        <v>136.397058</v>
+      </c>
+      <c r="C35">
+        <v>9.208651</v>
+      </c>
+      <c r="D35">
+        <v>12.60344</v>
+      </c>
+      <c r="E35">
+        <v>14.988</v>
+      </c>
+      <c r="F35">
+        <v>29.206577</v>
+      </c>
+      <c r="G35">
+        <v>31.019842</v>
+      </c>
+      <c r="H35">
+        <v>35.279024</v>
+      </c>
+      <c r="I35">
+        <v>29.089595</v>
+      </c>
+      <c r="J35">
+        <v>34.866216</v>
+      </c>
+      <c r="K35">
+        <v>51.784182</v>
+      </c>
+      <c r="L35">
+        <v>29.081075</v>
+      </c>
+      <c r="M35">
+        <v>33.753295</v>
+      </c>
+      <c r="N35">
+        <v>22.976343</v>
+      </c>
+      <c r="O35">
+        <v>17.174625</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B36">
+        <v>7.22915</v>
+      </c>
+      <c r="C36">
+        <v>0.437328</v>
+      </c>
+      <c r="D36">
+        <v>0.642215</v>
+      </c>
+      <c r="E36">
+        <v>0.783697</v>
+      </c>
+      <c r="F36">
+        <v>0.987318</v>
+      </c>
+      <c r="G36">
+        <v>0.903218</v>
+      </c>
+      <c r="H36">
+        <v>1.002007</v>
+      </c>
+      <c r="I36">
+        <v>1.124162</v>
+      </c>
+      <c r="J36">
+        <v>1.226224</v>
+      </c>
+      <c r="K36">
+        <v>1.277487</v>
+      </c>
+      <c r="L36">
+        <v>0.808388</v>
+      </c>
+      <c r="M36">
+        <v>1.021388</v>
+      </c>
+      <c r="N36">
+        <v>0.888037</v>
+      </c>
+      <c r="O36">
+        <v>0.602831</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B37">
+        <v>0.213655</v>
+      </c>
+      <c r="C37">
+        <v>2.162474</v>
+      </c>
+      <c r="D37">
+        <v>1.475236</v>
+      </c>
+      <c r="E37">
+        <v>1.894219</v>
+      </c>
+      <c r="F37">
+        <v>1.575682</v>
+      </c>
+      <c r="G37">
+        <v>1.453825</v>
+      </c>
+      <c r="H37">
+        <v>1.357417</v>
+      </c>
+      <c r="I37">
+        <v>1.36287</v>
+      </c>
+      <c r="J37">
+        <v>1.027371</v>
+      </c>
+      <c r="K37">
+        <v>1.104214</v>
+      </c>
+      <c r="L37">
+        <v>1.129274</v>
+      </c>
+      <c r="M37">
+        <v>1.18225</v>
+      </c>
+      <c r="N37">
+        <v>1.05644</v>
+      </c>
+      <c r="O37">
+        <v>1.309556</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B38">
+        <v>-3.506078</v>
+      </c>
+      <c r="C38">
+        <v>-0.01398</v>
+      </c>
+      <c r="D38">
+        <v>-0.143626</v>
+      </c>
+      <c r="E38">
+        <v>-2.643832</v>
+      </c>
+      <c r="F38">
+        <v>-1.59112</v>
+      </c>
+      <c r="G38">
+        <v>-0.936161</v>
+      </c>
+      <c r="H38">
+        <v>-0.91527</v>
+      </c>
+      <c r="I38">
+        <v>-0.698839</v>
+      </c>
+      <c r="J38">
+        <v>-1.506162</v>
+      </c>
+      <c r="K38">
+        <v>-1.837969</v>
+      </c>
+      <c r="L38">
+        <v>-1.78083</v>
+      </c>
+      <c r="M38">
+        <v>-1.988266</v>
+      </c>
+      <c r="N38">
+        <v>-1.877495</v>
+      </c>
+      <c r="O38">
+        <v>-0.936342</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B39">
+        <v>-5.487099</v>
+      </c>
+      <c r="C39">
+        <v>-0.016713</v>
+      </c>
+      <c r="D39">
+        <v>-0.173364</v>
+      </c>
+      <c r="E39">
+        <v>-3.659322</v>
+      </c>
+      <c r="F39">
+        <v>-2.262836</v>
+      </c>
+      <c r="G39">
+        <v>-1.133957</v>
+      </c>
+      <c r="H39">
+        <v>-1.161817</v>
+      </c>
+      <c r="I39">
+        <v>-1.092055</v>
+      </c>
+      <c r="J39">
+        <v>-1.94858</v>
+      </c>
+      <c r="K39">
+        <v>-2.458031</v>
+      </c>
+      <c r="L39">
+        <v>-2.701878</v>
+      </c>
+      <c r="M39">
+        <v>-2.508951</v>
+      </c>
+      <c r="N39">
+        <v>-2.248126</v>
+      </c>
+      <c r="O39">
+        <v>-1.113346</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="45.7109375" customWidth="1"/>
+    <col min="2" max="34" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2012</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2013</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2014</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2016</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2017</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2018</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="L1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="M1" s="1">
+        <v>2023</v>
+      </c>
+      <c r="N1" s="1">
+        <v>2024</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B27">
+        <v>20025</v>
+      </c>
+      <c r="C27">
+        <v>34517</v>
+      </c>
+      <c r="D27">
+        <v>52504</v>
+      </c>
+      <c r="E27">
+        <v>76204</v>
+      </c>
+      <c r="F27">
+        <v>101143</v>
+      </c>
+      <c r="G27">
+        <v>158273</v>
+      </c>
+      <c r="H27">
+        <v>250266</v>
+      </c>
+      <c r="I27">
+        <v>376844</v>
+      </c>
+      <c r="J27">
+        <v>509711</v>
+      </c>
+      <c r="K27">
+        <v>717289</v>
+      </c>
+      <c r="L27">
+        <v>853062</v>
+      </c>
+      <c r="M27">
+        <v>868687</v>
+      </c>
+      <c r="N27">
+        <v>941168</v>
+      </c>
+      <c r="O27">
+        <v>981767</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B28">
+        <v>13471</v>
+      </c>
+      <c r="C28">
+        <v>24798</v>
+      </c>
+      <c r="D28">
+        <v>39135</v>
+      </c>
+      <c r="E28">
+        <v>52370</v>
+      </c>
+      <c r="F28">
+        <v>66788</v>
+      </c>
+      <c r="G28">
+        <v>99647</v>
+      </c>
+      <c r="H28">
+        <v>144023</v>
+      </c>
+      <c r="I28">
+        <v>172758</v>
+      </c>
+      <c r="J28">
+        <v>229998</v>
+      </c>
+      <c r="K28">
+        <v>297772</v>
+      </c>
+      <c r="L28">
+        <v>314357</v>
+      </c>
+      <c r="M28">
+        <v>320125</v>
+      </c>
+      <c r="N28">
+        <v>354845</v>
+      </c>
+      <c r="O28">
+        <v>381010</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B29">
+        <v>6005</v>
+      </c>
+      <c r="C29">
+        <v>15307</v>
+      </c>
+      <c r="D29">
+        <v>27843</v>
+      </c>
+      <c r="E29">
+        <v>27765</v>
+      </c>
+      <c r="F29">
+        <v>36534</v>
+      </c>
+      <c r="G29">
+        <v>63097</v>
+      </c>
+      <c r="H29">
+        <v>92494</v>
+      </c>
+      <c r="I29">
+        <v>98542</v>
+      </c>
+      <c r="J29">
+        <v>137763</v>
+      </c>
+      <c r="K29">
+        <v>157503</v>
+      </c>
+      <c r="L29">
+        <v>144562</v>
+      </c>
+      <c r="M29">
+        <v>153947</v>
+      </c>
+      <c r="N29">
+        <v>183222</v>
+      </c>
+      <c r="O29">
+        <v>190468</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B30">
+        <v>5150</v>
+      </c>
+      <c r="C30">
+        <v>14413</v>
+      </c>
+      <c r="D30">
+        <v>26233</v>
+      </c>
+      <c r="E30">
+        <v>23310</v>
+      </c>
+      <c r="F30">
+        <v>29557</v>
+      </c>
+      <c r="G30">
+        <v>48912</v>
+      </c>
+      <c r="H30">
+        <v>70609</v>
+      </c>
+      <c r="I30">
+        <v>61606</v>
+      </c>
+      <c r="J30">
+        <v>95534</v>
+      </c>
+      <c r="K30">
+        <v>109594</v>
+      </c>
+      <c r="L30">
+        <v>96497</v>
+      </c>
+      <c r="M30">
+        <v>107009</v>
+      </c>
+      <c r="N30">
+        <v>138718</v>
+      </c>
+      <c r="O30">
+        <v>148223</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B32">
+        <v>12.560271</v>
+      </c>
+      <c r="C32">
+        <v>-0.011033</v>
+      </c>
+      <c r="D32">
+        <v>13.174896</v>
+      </c>
+      <c r="E32">
+        <v>58.280527</v>
+      </c>
+      <c r="F32">
+        <v>87.709509</v>
+      </c>
+      <c r="G32">
+        <v>110.197233</v>
+      </c>
+      <c r="H32">
+        <v>142.899218</v>
+      </c>
+      <c r="I32">
+        <v>190.276638</v>
+      </c>
+      <c r="J32">
+        <v>281.184134</v>
+      </c>
+      <c r="K32">
+        <v>345.626486</v>
+      </c>
+      <c r="L32">
+        <v>355.280105</v>
+      </c>
+      <c r="M32">
+        <v>385.718073</v>
+      </c>
+      <c r="N32">
+        <v>405.377807</v>
+      </c>
+      <c r="O32">
+        <v>432.523194</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B33">
+        <v>7.178437</v>
+      </c>
+      <c r="C33">
+        <v>-6.227873</v>
+      </c>
+      <c r="D33">
+        <v>6.277588</v>
+      </c>
+      <c r="E33">
+        <v>37.598091</v>
+      </c>
+      <c r="F33">
+        <v>51.374173</v>
+      </c>
+      <c r="G33">
+        <v>53.193675</v>
+      </c>
+      <c r="H33">
+        <v>65.168359</v>
+      </c>
+      <c r="I33">
+        <v>58.996322</v>
+      </c>
+      <c r="J33">
+        <v>155.470723</v>
+      </c>
+      <c r="K33">
+        <v>211.572945</v>
+      </c>
+      <c r="L33">
+        <v>232.114107</v>
+      </c>
+      <c r="M33">
+        <v>262.9455</v>
+      </c>
+      <c r="N33">
+        <v>287.599953</v>
+      </c>
+      <c r="O33">
+        <v>313.017011</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>